<commit_message>
redone a lot to make test case full run
</commit_message>
<xml_diff>
--- a/input/forces.xlsx
+++ b/input/forces.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\source\repos\Debugging-Li2SO4\Old experiments passed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\source\repos\Debugging-Li2SO4\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE15EDA-2879-4AC7-8064-22D678B90283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF623B6-5EE6-4736-832A-55DD32E6032F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="2" xr2:uid="{874B0134-1390-4BF3-83C4-416E653BC7FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{874B0134-1390-4BF3-83C4-416E653BC7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Li-Li</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Experimental</t>
+  </si>
+  <si>
+    <t>T= 323.15</t>
   </si>
 </sst>
 </file>
@@ -503,13 +506,13 @@
       <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="17.5703125" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" customWidth="1"/>
+    <col min="3" max="4" width="17.54296875" customWidth="1"/>
+    <col min="6" max="7" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -523,7 +526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -534,7 +537,7 @@
         <v>3.1589</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -553,7 +556,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -572,7 +575,7 @@
         <v>3.3544499999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -591,7 +594,7 @@
         <v>3.4044499999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -610,7 +613,7 @@
         <v>1.4396999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -629,7 +632,7 @@
         <v>2.4948499999999996</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -648,7 +651,7 @@
         <v>2.8448500000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -667,7 +670,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -686,7 +689,7 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -705,7 +708,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
@@ -718,16 +721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CDAB35-1A88-4732-A8F7-3C43358ED72A}">
   <dimension ref="B4:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="31.42578125" customWidth="1"/>
+    <col min="11" max="11" width="31.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>15</v>
       </c>
@@ -753,7 +756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
@@ -780,7 +783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
@@ -807,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>3</v>
       </c>
@@ -834,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>4</v>
       </c>
@@ -861,7 +864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>5</v>
       </c>
@@ -891,7 +894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>6</v>
       </c>
@@ -927,29 +930,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855CDA98-50B5-463D-99EB-A9AEFFC97778}">
   <dimension ref="A2:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -977,7 +980,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1011,7 +1014,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1039,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1233,18 +1236,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1267,14 +1270,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34AC1221-5A6C-4F6B-98AA-6C97E1E179EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68C28FD1-FDAB-4FA6-AACF-841A9330F756}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1289,4 +1284,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34AC1221-5A6C-4F6B-98AA-6C97E1E179EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>